<commit_message>
update loc_holiday.xlsx column names
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/loc_holiday.xlsx
+++ b/mosip_master/xlsx/loc_holiday.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-sln\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E8481A-0E2B-4457-AA48-55D32741F1C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F51FDA-4AF6-4D5E-AF63-F3700481F0D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{33038397-233E-4B60-B19D-1D8B5E63155B}"/>
   </bookViews>
@@ -26,9 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="15">
-  <si>
-    <t>langCode</t>
-  </si>
   <si>
     <t>SLE</t>
   </si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>is_active</t>
+  </si>
+  <si>
+    <t>lang_code</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,45 +453,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>2000001</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <v>44927</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -499,22 +499,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>2000002</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
         <v>44933</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -522,22 +522,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>2000003</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>44934</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -545,22 +545,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>2000004</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
         <v>44940</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -568,22 +568,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2000005</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
         <v>44941</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -591,22 +591,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>2000006</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <v>44947</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -614,22 +614,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>2000007</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
         <v>44948</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -637,22 +637,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>2000008</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <v>44954</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -660,22 +660,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>2000009</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <v>44955</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -683,22 +683,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>2000010</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
         <v>44961</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -706,22 +706,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>2000011</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>44962</v>
       </c>
       <c r="E12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -729,22 +729,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>2000012</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>44968</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
@@ -752,22 +752,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>2000013</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>44969</v>
       </c>
       <c r="E14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
@@ -775,22 +775,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>2000014</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
         <v>44975</v>
       </c>
       <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
@@ -798,22 +798,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <v>2000015</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" s="1">
         <v>44976</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
@@ -821,22 +821,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
         <v>2000016</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="1">
         <v>44982</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
@@ -844,22 +844,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>2000017</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="1">
         <v>44983</v>
       </c>
       <c r="E18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
@@ -867,22 +867,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <v>2000018</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <v>44989</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
@@ -890,22 +890,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>2000019</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
         <v>44990</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
@@ -913,22 +913,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21">
         <v>2000020</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="1">
         <v>44993</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G21" t="b">
         <v>1</v>
@@ -936,22 +936,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>2000021</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
         <v>44996</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22" t="b">
         <v>1</v>
@@ -959,22 +959,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23">
         <v>2000022</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
         <v>44997</v>
       </c>
       <c r="E23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G23" t="b">
         <v>1</v>
@@ -982,22 +982,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>2000023</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
         <v>45003</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" t="b">
         <v>1</v>
@@ -1005,22 +1005,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25">
         <v>2000024</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1">
         <v>45004</v>
       </c>
       <c r="E25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G25" t="b">
         <v>1</v>
@@ -1028,22 +1028,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26">
         <v>2000025</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
         <v>45010</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
@@ -1051,22 +1051,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27">
         <v>2000026</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1">
         <v>45011</v>
       </c>
       <c r="E27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
@@ -1074,22 +1074,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28">
         <v>2000027</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1">
         <v>45017</v>
       </c>
       <c r="E28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G28" t="b">
         <v>1</v>
@@ -1097,22 +1097,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29">
         <v>2000028</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
         <v>45018</v>
       </c>
       <c r="E29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29" t="b">
         <v>1</v>
@@ -1120,22 +1120,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B30">
         <v>2000029</v>
       </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
         <v>45024</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G30" t="b">
         <v>1</v>
@@ -1143,22 +1143,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B31">
         <v>2000030</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
         <v>45025</v>
       </c>
       <c r="E31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G31" t="b">
         <v>1</v>
@@ -1166,22 +1166,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32">
         <v>2000031</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="1">
         <v>45031</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G32" t="b">
         <v>1</v>
@@ -1189,22 +1189,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33">
         <v>2000032</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="1">
         <v>45032</v>
       </c>
       <c r="E33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G33" t="b">
         <v>1</v>
@@ -1212,22 +1212,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34">
         <v>2000033</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
         <v>45038</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34" t="b">
         <v>1</v>
@@ -1235,22 +1235,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>2000034</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="1">
         <v>45039</v>
       </c>
       <c r="E35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
@@ -1258,22 +1258,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B36">
         <v>2000035</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" s="1">
         <v>45045</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G36" t="b">
         <v>1</v>
@@ -1281,22 +1281,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>2000036</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" s="1">
         <v>45046</v>
       </c>
       <c r="E37" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G37" t="b">
         <v>1</v>
@@ -1304,22 +1304,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>2000037</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="1">
         <v>45052</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38" t="b">
         <v>1</v>
@@ -1327,22 +1327,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39">
         <v>2000038</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="1">
         <v>45053</v>
       </c>
       <c r="E39" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" t="b">
         <v>1</v>
@@ -1350,22 +1350,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40">
         <v>2000039</v>
       </c>
       <c r="C40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <v>45059</v>
       </c>
       <c r="E40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G40" t="b">
         <v>1</v>
@@ -1373,22 +1373,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41">
         <v>2000040</v>
       </c>
       <c r="C41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="1">
         <v>45060</v>
       </c>
       <c r="E41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41" t="b">
         <v>1</v>
@@ -1396,22 +1396,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42">
         <v>2000041</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="1">
         <v>45066</v>
       </c>
       <c r="E42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G42" t="b">
         <v>1</v>
@@ -1419,22 +1419,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B43">
         <v>2000042</v>
       </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="1">
         <v>45067</v>
       </c>
       <c r="E43" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G43" t="b">
         <v>1</v>
@@ -1442,22 +1442,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B44">
         <v>2000043</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="1">
         <v>45073</v>
       </c>
       <c r="E44" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G44" t="b">
         <v>1</v>
@@ -1465,22 +1465,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B45">
         <v>2000044</v>
       </c>
       <c r="C45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="1">
         <v>45074</v>
       </c>
       <c r="E45" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G45" t="b">
         <v>1</v>
@@ -1488,22 +1488,22 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46">
         <v>2000045</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="1">
         <v>45080</v>
       </c>
       <c r="E46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F46" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G46" t="b">
         <v>1</v>
@@ -1511,22 +1511,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47">
         <v>2000046</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="1">
         <v>45081</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" t="b">
         <v>1</v>
@@ -1534,22 +1534,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B48">
         <v>2000047</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="1">
         <v>45087</v>
       </c>
       <c r="E48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G48" t="b">
         <v>1</v>
@@ -1557,22 +1557,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B49">
         <v>2000048</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="1">
         <v>45088</v>
       </c>
       <c r="E49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G49" t="b">
         <v>1</v>
@@ -1580,22 +1580,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B50">
         <v>2000049</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="1">
         <v>45094</v>
       </c>
       <c r="E50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50" t="b">
         <v>1</v>
@@ -1603,22 +1603,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B51">
         <v>2000050</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="1">
         <v>45095</v>
       </c>
       <c r="E51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G51" t="b">
         <v>1</v>
@@ -1626,22 +1626,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B52">
         <v>2000051</v>
       </c>
       <c r="C52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="1">
         <v>45101</v>
       </c>
       <c r="E52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F52" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G52" t="b">
         <v>1</v>
@@ -1649,22 +1649,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B53">
         <v>2000052</v>
       </c>
       <c r="C53" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="1">
         <v>45102</v>
       </c>
       <c r="E53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G53" t="b">
         <v>1</v>
@@ -1672,22 +1672,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B54">
         <v>2000053</v>
       </c>
       <c r="C54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="1">
         <v>45108</v>
       </c>
       <c r="E54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F54" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G54" t="b">
         <v>1</v>
@@ -1695,22 +1695,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B55">
         <v>2000054</v>
       </c>
       <c r="C55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="1">
         <v>45109</v>
       </c>
       <c r="E55" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G55" t="b">
         <v>1</v>
@@ -1718,22 +1718,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B56">
         <v>2000055</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="1">
         <v>45115</v>
       </c>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G56" t="b">
         <v>1</v>
@@ -1741,22 +1741,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B57">
         <v>2000056</v>
       </c>
       <c r="C57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" s="1">
         <v>45116</v>
       </c>
       <c r="E57" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G57" t="b">
         <v>1</v>
@@ -1764,22 +1764,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B58">
         <v>2000057</v>
       </c>
       <c r="C58" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" s="1">
         <v>45122</v>
       </c>
       <c r="E58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G58" t="b">
         <v>1</v>
@@ -1787,22 +1787,22 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B59">
         <v>2000058</v>
       </c>
       <c r="C59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" s="1">
         <v>45123</v>
       </c>
       <c r="E59" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G59" t="b">
         <v>1</v>
@@ -1810,22 +1810,22 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B60">
         <v>2000059</v>
       </c>
       <c r="C60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D60" s="1">
         <v>45129</v>
       </c>
       <c r="E60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F60" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G60" t="b">
         <v>1</v>
@@ -1833,22 +1833,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B61">
         <v>2000060</v>
       </c>
       <c r="C61" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61" s="1">
         <v>45130</v>
       </c>
       <c r="E61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G61" t="b">
         <v>1</v>
@@ -1856,22 +1856,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B62">
         <v>2000061</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" s="1">
         <v>45136</v>
       </c>
       <c r="E62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G62" t="b">
         <v>1</v>
@@ -1879,22 +1879,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B63">
         <v>2000062</v>
       </c>
       <c r="C63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="1">
         <v>45137</v>
       </c>
       <c r="E63" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G63" t="b">
         <v>1</v>
@@ -1902,22 +1902,22 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B64">
         <v>2000063</v>
       </c>
       <c r="C64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64" s="1">
         <v>45143</v>
       </c>
       <c r="E64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F64" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G64" t="b">
         <v>1</v>
@@ -1925,22 +1925,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B65">
         <v>2000064</v>
       </c>
       <c r="C65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D65" s="1">
         <v>45144</v>
       </c>
       <c r="E65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G65" t="b">
         <v>1</v>
@@ -1948,22 +1948,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B66">
         <v>2000065</v>
       </c>
       <c r="C66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" s="1">
         <v>45150</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F66" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G66" t="b">
         <v>1</v>
@@ -1971,22 +1971,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B67">
         <v>2000066</v>
       </c>
       <c r="C67" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67" s="1">
         <v>45151</v>
       </c>
       <c r="E67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G67" t="b">
         <v>1</v>
@@ -1994,22 +1994,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B68">
         <v>2000067</v>
       </c>
       <c r="C68" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="1">
         <v>45157</v>
       </c>
       <c r="E68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F68" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G68" t="b">
         <v>1</v>
@@ -2017,22 +2017,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B69">
         <v>2000068</v>
       </c>
       <c r="C69" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="1">
         <v>45158</v>
       </c>
       <c r="E69" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G69" t="b">
         <v>1</v>
@@ -2040,22 +2040,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B70">
         <v>2000069</v>
       </c>
       <c r="C70" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="1">
         <v>45164</v>
       </c>
       <c r="E70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G70" t="b">
         <v>1</v>
@@ -2063,22 +2063,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71">
         <v>2000070</v>
       </c>
       <c r="C71" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" s="1">
         <v>45165</v>
       </c>
       <c r="E71" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G71" t="b">
         <v>1</v>
@@ -2086,22 +2086,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B72">
         <v>2000071</v>
       </c>
       <c r="C72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="1">
         <v>45171</v>
       </c>
       <c r="E72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G72" t="b">
         <v>1</v>
@@ -2109,22 +2109,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B73">
         <v>2000072</v>
       </c>
       <c r="C73" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" s="1">
         <v>45172</v>
       </c>
       <c r="E73" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G73" t="b">
         <v>1</v>
@@ -2132,22 +2132,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B74">
         <v>2000073</v>
       </c>
       <c r="C74" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="1">
         <v>45178</v>
       </c>
       <c r="E74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F74" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G74" t="b">
         <v>1</v>
@@ -2155,22 +2155,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B75">
         <v>2000074</v>
       </c>
       <c r="C75" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" s="1">
         <v>45179</v>
       </c>
       <c r="E75" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G75" t="b">
         <v>1</v>
@@ -2178,22 +2178,22 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B76">
         <v>2000075</v>
       </c>
       <c r="C76" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" s="1">
         <v>45185</v>
       </c>
       <c r="E76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G76" t="b">
         <v>1</v>
@@ -2201,22 +2201,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B77">
         <v>2000076</v>
       </c>
       <c r="C77" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" s="1">
         <v>45186</v>
       </c>
       <c r="E77" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G77" t="b">
         <v>1</v>
@@ -2224,22 +2224,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B78">
         <v>2000077</v>
       </c>
       <c r="C78" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" s="1">
         <v>45192</v>
       </c>
       <c r="E78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F78" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G78" t="b">
         <v>1</v>
@@ -2247,22 +2247,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B79">
         <v>2000078</v>
       </c>
       <c r="C79" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="1">
         <v>45193</v>
       </c>
       <c r="E79" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G79" t="b">
         <v>1</v>
@@ -2270,22 +2270,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B80">
         <v>2000079</v>
       </c>
       <c r="C80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" s="1">
         <v>45199</v>
       </c>
       <c r="E80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G80" t="b">
         <v>1</v>
@@ -2293,22 +2293,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B81">
         <v>2000080</v>
       </c>
       <c r="C81" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" s="1">
         <v>45200</v>
       </c>
       <c r="E81" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
@@ -2316,22 +2316,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B82">
         <v>2000081</v>
       </c>
       <c r="C82" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="1">
         <v>45206</v>
       </c>
       <c r="E82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G82" t="b">
         <v>1</v>
@@ -2339,22 +2339,22 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B83">
         <v>2000082</v>
       </c>
       <c r="C83" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" s="1">
         <v>45207</v>
       </c>
       <c r="E83" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G83" t="b">
         <v>1</v>
@@ -2362,22 +2362,22 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B84">
         <v>2000083</v>
       </c>
       <c r="C84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" s="1">
         <v>45213</v>
       </c>
       <c r="E84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G84" t="b">
         <v>1</v>
@@ -2385,22 +2385,22 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B85">
         <v>2000084</v>
       </c>
       <c r="C85" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" s="1">
         <v>45214</v>
       </c>
       <c r="E85" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G85" t="b">
         <v>1</v>
@@ -2408,22 +2408,22 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B86">
         <v>2000085</v>
       </c>
       <c r="C86" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="1">
         <v>45220</v>
       </c>
       <c r="E86" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G86" t="b">
         <v>1</v>
@@ -2431,22 +2431,22 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B87">
         <v>2000086</v>
       </c>
       <c r="C87" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" s="1">
         <v>45221</v>
       </c>
       <c r="E87" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G87" t="b">
         <v>1</v>
@@ -2454,22 +2454,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B88">
         <v>2000087</v>
       </c>
       <c r="C88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" s="1">
         <v>45227</v>
       </c>
       <c r="E88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G88" t="b">
         <v>1</v>
@@ -2477,22 +2477,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B89">
         <v>2000088</v>
       </c>
       <c r="C89" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" s="1">
         <v>45228</v>
       </c>
       <c r="E89" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G89" t="b">
         <v>1</v>
@@ -2500,22 +2500,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B90">
         <v>2000089</v>
       </c>
       <c r="C90" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" s="1">
         <v>45234</v>
       </c>
       <c r="E90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G90" t="b">
         <v>1</v>
@@ -2523,22 +2523,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B91">
         <v>2000090</v>
       </c>
       <c r="C91" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" s="1">
         <v>45235</v>
       </c>
       <c r="E91" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G91" t="b">
         <v>1</v>
@@ -2546,22 +2546,22 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B92">
         <v>2000091</v>
       </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" s="1">
         <v>45241</v>
       </c>
       <c r="E92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F92" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G92" t="b">
         <v>1</v>
@@ -2569,22 +2569,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B93">
         <v>2000092</v>
       </c>
       <c r="C93" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93" s="1">
         <v>45242</v>
       </c>
       <c r="E93" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G93" t="b">
         <v>1</v>
@@ -2592,22 +2592,22 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B94">
         <v>2000093</v>
       </c>
       <c r="C94" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" s="1">
         <v>45248</v>
       </c>
       <c r="E94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F94" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G94" t="b">
         <v>1</v>
@@ -2615,22 +2615,22 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B95">
         <v>2000094</v>
       </c>
       <c r="C95" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" s="1">
         <v>45249</v>
       </c>
       <c r="E95" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G95" t="b">
         <v>1</v>
@@ -2638,22 +2638,22 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B96">
         <v>2000095</v>
       </c>
       <c r="C96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" s="1">
         <v>45255</v>
       </c>
       <c r="E96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F96" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G96" t="b">
         <v>1</v>
@@ -2661,22 +2661,22 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B97">
         <v>2000096</v>
       </c>
       <c r="C97" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97" s="1">
         <v>45256</v>
       </c>
       <c r="E97" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G97" t="b">
         <v>1</v>
@@ -2684,22 +2684,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B98">
         <v>2000097</v>
       </c>
       <c r="C98" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" s="1">
         <v>45262</v>
       </c>
       <c r="E98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F98" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G98" t="b">
         <v>1</v>
@@ -2707,22 +2707,22 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B99">
         <v>2000098</v>
       </c>
       <c r="C99" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" s="1">
         <v>45263</v>
       </c>
       <c r="E99" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G99" t="b">
         <v>1</v>
@@ -2730,22 +2730,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B100">
         <v>2000099</v>
       </c>
       <c r="C100" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" s="1">
         <v>45269</v>
       </c>
       <c r="E100" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G100" t="b">
         <v>1</v>
@@ -2753,22 +2753,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B101">
         <v>2000100</v>
       </c>
       <c r="C101" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="1">
         <v>45270</v>
       </c>
       <c r="E101" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G101" t="b">
         <v>1</v>
@@ -2776,22 +2776,22 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B102">
         <v>2000101</v>
       </c>
       <c r="C102" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102" s="1">
         <v>45276</v>
       </c>
       <c r="E102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F102" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G102" t="b">
         <v>1</v>
@@ -2799,22 +2799,22 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B103">
         <v>2000102</v>
       </c>
       <c r="C103" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" s="1">
         <v>45277</v>
       </c>
       <c r="E103" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G103" t="b">
         <v>1</v>
@@ -2822,22 +2822,22 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B104">
         <v>2000103</v>
       </c>
       <c r="C104" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104" s="1">
         <v>45283</v>
       </c>
       <c r="E104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F104" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G104" t="b">
         <v>1</v>
@@ -2845,22 +2845,22 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B105">
         <v>2000104</v>
       </c>
       <c r="C105" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D105" s="1">
         <v>45284</v>
       </c>
       <c r="E105" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F105" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G105" t="b">
         <v>1</v>
@@ -2868,22 +2868,22 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B106">
         <v>2000105</v>
       </c>
       <c r="C106" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" s="1">
         <v>45290</v>
       </c>
       <c r="E106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F106" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G106" t="b">
         <v>1</v>
@@ -2891,22 +2891,22 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B107">
         <v>2000106</v>
       </c>
       <c r="C107" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107" s="1">
         <v>45291</v>
       </c>
       <c r="E107" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" t="b">
         <v>1</v>

</xml_diff>